<commit_message>
Add weight to household surplus
and fix plotting functions
</commit_message>
<xml_diff>
--- a/model/Outputs/8. Fixed RE/No PV w Bat/Evaluation Metrics.xlsx
+++ b/model/Outputs/8. Fixed RE/No PV w Bat/Evaluation Metrics.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/Model-1/model/Outputs/8. Fixed RE/No PV w Bat/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_D0156514CA30921FD2FE31D2F8F2D3C284D5BE6D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{064AF741-989F-4649-A936-AE221BC646E3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -64,8 +58,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,21 +122,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -180,7 +166,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -214,7 +200,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -249,10 +234,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -425,23 +409,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -461,144 +436,144 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="C2">
-        <v>0.28000000000000003</v>
+        <v>0.31</v>
       </c>
       <c r="D2">
-        <v>3.6153411390026487E-2</v>
+        <v>0.1456984653693756</v>
       </c>
       <c r="E2">
-        <v>0.1919045416885283</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>676024.24307209905</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1494365305.884841</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="C3">
-        <v>0.28000000000000003</v>
+        <v>0.31</v>
       </c>
       <c r="D3">
-        <v>3.6153411390004747E-2</v>
+        <v>0.1448620987924807</v>
       </c>
       <c r="E3">
-        <v>0.1919045416885285</v>
+        <v>2.625002048089096E-17</v>
       </c>
       <c r="F3">
-        <v>676024.24307209405</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1494370764.077965</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="C4">
-        <v>0.28000000000000003</v>
+        <v>0.31</v>
       </c>
       <c r="D4">
-        <v>3.6153411390024127E-2</v>
+        <v>0.1456984653691645</v>
       </c>
       <c r="E4">
-        <v>0.19190454168852841</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>676024.24307209905</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1494365305.884843</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="C5">
-        <v>0.28000000000000003</v>
+        <v>0.31</v>
       </c>
       <c r="D5">
-        <v>3.6153411390024127E-2</v>
+        <v>0.1456984653690596</v>
       </c>
       <c r="E5">
-        <v>0.1919045416885285</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>676024.24307209894</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1494365305.884843</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.3</v>
+        <v>0.02</v>
       </c>
       <c r="C6">
-        <v>0.28000000000000003</v>
+        <v>0.31</v>
       </c>
       <c r="D6">
-        <v>0.54329584107268269</v>
+        <v>0.1448620987924807</v>
       </c>
       <c r="E6">
-        <v>0.77358938355156293</v>
+        <v>2.625002048089096E-17</v>
       </c>
       <c r="F6">
-        <v>725509.82704385766</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1494370764.077965</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.3</v>
+        <v>0.02</v>
       </c>
       <c r="C7">
-        <v>0.28000000000000003</v>
+        <v>0.31</v>
       </c>
       <c r="D7">
-        <v>0.61871972628331751</v>
+        <v>0.1448620987924808</v>
       </c>
       <c r="E7">
-        <v>0.7383053495558678</v>
+        <v>1.852942622180538E-17</v>
       </c>
       <c r="F7">
-        <v>766939.0524050981</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1494370764.077965</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>0.28000000000000003</v>
+        <v>0.31</v>
       </c>
       <c r="D8">
-        <v>0.74867945921166013</v>
+        <v>0.2269628541449643</v>
       </c>
       <c r="E8">
-        <v>0.80560296672229903</v>
+        <v>1.544118851817115E-17</v>
       </c>
       <c r="F8">
-        <v>796177.71600184881</v>
+        <v>1493530195.173004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>